<commit_message>
Angebot, Projektzeitplan wurden angepasst
spUpdate-  und spDeleteImage wurden angepasst
</commit_message>
<xml_diff>
--- a/Docs/Zeichnungen/Projektzeitplan.xlsx
+++ b/Docs/Zeichnungen/Projektzeitplan.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
   </bookViews>
   <sheets>
     <sheet name="Projektzeitplan" sheetId="8" r:id="rId1"/>
@@ -329,7 +329,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -351,41 +351,47 @@
     <xf numFmtId="14" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -733,8 +739,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -761,10 +767,10 @@
       <c r="A2" s="1"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="14">
+      <c r="E2" s="11">
         <f>DATE(2025,2,3)</f>
         <v>45691</v>
       </c>
@@ -792,11 +798,11 @@
       <c r="D4" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="E4" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
@@ -824,7 +830,7 @@
       <c r="B6" s="2">
         <v>1</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="20" t="s">
         <v>17</v>
       </c>
       <c r="D6" s="2" t="s">
@@ -836,7 +842,7 @@
       <c r="F6" s="2">
         <v>8</v>
       </c>
-      <c r="G6" s="16" t="s">
+      <c r="G6" s="13" t="s">
         <v>8</v>
       </c>
     </row>
@@ -845,7 +851,7 @@
       <c r="B7" s="2">
         <v>2</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="20" t="s">
         <v>18</v>
       </c>
       <c r="D7" s="2" t="s">
@@ -857,7 +863,7 @@
       <c r="F7" s="2">
         <v>6</v>
       </c>
-      <c r="G7" s="16" t="s">
+      <c r="G7" s="13" t="s">
         <v>8</v>
       </c>
     </row>
@@ -866,7 +872,7 @@
       <c r="B8" s="2">
         <v>3</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="20" t="s">
         <v>19</v>
       </c>
       <c r="D8" s="2" t="s">
@@ -878,7 +884,7 @@
       <c r="F8" s="2">
         <v>7</v>
       </c>
-      <c r="G8" s="16" t="s">
+      <c r="G8" s="13" t="s">
         <v>8</v>
       </c>
     </row>
@@ -887,7 +893,7 @@
       <c r="B9" s="2">
         <v>4</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="20" t="s">
         <v>20</v>
       </c>
       <c r="D9" s="2" t="s">
@@ -899,7 +905,7 @@
       <c r="F9" s="2">
         <v>7</v>
       </c>
-      <c r="G9" s="16" t="s">
+      <c r="G9" s="13" t="s">
         <v>8</v>
       </c>
     </row>
@@ -908,7 +914,7 @@
       <c r="B10" s="2">
         <v>5</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="20" t="s">
         <v>21</v>
       </c>
       <c r="D10" s="2" t="s">
@@ -920,7 +926,7 @@
       <c r="F10" s="2">
         <v>6</v>
       </c>
-      <c r="G10" s="16" t="s">
+      <c r="G10" s="13" t="s">
         <v>8</v>
       </c>
     </row>
@@ -929,7 +935,7 @@
       <c r="B11" s="2">
         <v>6</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="20" t="s">
         <v>22</v>
       </c>
       <c r="D11" s="2" t="s">
@@ -941,7 +947,7 @@
       <c r="F11" s="2">
         <v>7</v>
       </c>
-      <c r="G11" s="16" t="s">
+      <c r="G11" s="13" t="s">
         <v>8</v>
       </c>
     </row>
@@ -950,7 +956,7 @@
       <c r="B12" s="2">
         <v>7</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="20" t="s">
         <v>23</v>
       </c>
       <c r="D12" s="2" t="s">
@@ -962,7 +968,7 @@
       <c r="F12" s="2">
         <v>6</v>
       </c>
-      <c r="G12" s="16" t="s">
+      <c r="G12" s="13" t="s">
         <v>8</v>
       </c>
     </row>
@@ -971,7 +977,7 @@
       <c r="B13" s="2">
         <v>8</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="20" t="s">
         <v>24</v>
       </c>
       <c r="D13" s="2" t="s">
@@ -983,7 +989,7 @@
       <c r="F13" s="2">
         <v>8</v>
       </c>
-      <c r="G13" s="16" t="s">
+      <c r="G13" s="13" t="s">
         <v>8</v>
       </c>
     </row>
@@ -992,7 +998,7 @@
       <c r="B14" s="2">
         <v>9</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C14" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D14" s="2" t="s">
@@ -1004,7 +1010,7 @@
       <c r="F14" s="2">
         <v>5</v>
       </c>
-      <c r="G14" s="16" t="s">
+      <c r="G14" s="13" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1013,7 +1019,7 @@
       <c r="B15" s="2">
         <v>10</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="C15" s="20" t="s">
         <v>26</v>
       </c>
       <c r="D15" s="2" t="s">
@@ -1025,7 +1031,7 @@
       <c r="F15" s="2">
         <v>7</v>
       </c>
-      <c r="G15" s="16" t="s">
+      <c r="G15" s="13" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1034,7 +1040,7 @@
       <c r="B16" s="2">
         <v>11</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="20" t="s">
         <v>27</v>
       </c>
       <c r="D16" s="2" t="s">
@@ -1046,7 +1052,7 @@
       <c r="F16" s="2">
         <v>8</v>
       </c>
-      <c r="G16" s="16" t="s">
+      <c r="G16" s="13" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1055,7 +1061,7 @@
       <c r="B17" s="2">
         <v>12</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="C17" s="20" t="s">
         <v>45</v>
       </c>
       <c r="D17" s="2" t="s">
@@ -1067,7 +1073,7 @@
       <c r="F17" s="2">
         <v>6</v>
       </c>
-      <c r="G17" s="16" t="s">
+      <c r="G17" s="13" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1076,7 +1082,7 @@
       <c r="B18" s="2">
         <v>13</v>
       </c>
-      <c r="C18" s="12" t="s">
+      <c r="C18" s="20" t="s">
         <v>29</v>
       </c>
       <c r="D18" s="2" t="s">
@@ -1088,7 +1094,7 @@
       <c r="F18" s="2">
         <v>8</v>
       </c>
-      <c r="G18" s="10" t="s">
+      <c r="G18" s="9" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1097,7 +1103,7 @@
       <c r="B19" s="2">
         <v>14</v>
       </c>
-      <c r="C19" s="12" t="s">
+      <c r="C19" s="20" t="s">
         <v>30</v>
       </c>
       <c r="D19" s="2" t="s">
@@ -1109,7 +1115,7 @@
       <c r="F19" s="2">
         <v>8</v>
       </c>
-      <c r="G19" s="10" t="s">
+      <c r="G19" s="9" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1118,7 +1124,7 @@
       <c r="B20" s="2">
         <v>15</v>
       </c>
-      <c r="C20" s="12" t="s">
+      <c r="C20" s="20" t="s">
         <v>40</v>
       </c>
       <c r="D20" s="2" t="s">
@@ -1130,7 +1136,7 @@
       <c r="F20" s="2">
         <v>8</v>
       </c>
-      <c r="G20" s="10" t="s">
+      <c r="G20" s="9" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1139,7 +1145,7 @@
       <c r="B21" s="2">
         <v>16</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="21" t="s">
         <v>41</v>
       </c>
       <c r="D21" s="2" t="s">
@@ -1151,7 +1157,7 @@
       <c r="F21" s="2">
         <v>8</v>
       </c>
-      <c r="G21" s="10" t="s">
+      <c r="G21" s="9" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1160,7 +1166,7 @@
       <c r="B22" s="2">
         <v>17</v>
       </c>
-      <c r="C22" s="12" t="s">
+      <c r="C22" s="20" t="s">
         <v>42</v>
       </c>
       <c r="D22" s="2" t="s">
@@ -1172,7 +1178,7 @@
       <c r="F22" s="2">
         <v>8</v>
       </c>
-      <c r="G22" s="10" t="s">
+      <c r="G22" s="9" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1181,7 +1187,7 @@
       <c r="B23" s="2">
         <v>18</v>
       </c>
-      <c r="C23" s="12" t="s">
+      <c r="C23" s="20" t="s">
         <v>43</v>
       </c>
       <c r="D23" s="2" t="s">
@@ -1193,7 +1199,7 @@
       <c r="F23" s="2">
         <v>7</v>
       </c>
-      <c r="G23" s="10" t="s">
+      <c r="G23" s="9" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1202,7 +1208,7 @@
       <c r="B24" s="2">
         <v>19</v>
       </c>
-      <c r="C24" s="12" t="s">
+      <c r="C24" s="20" t="s">
         <v>44</v>
       </c>
       <c r="D24" s="2" t="s">
@@ -1214,7 +1220,7 @@
       <c r="F24" s="2">
         <v>8</v>
       </c>
-      <c r="G24" s="10" t="s">
+      <c r="G24" s="9" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1223,7 +1229,7 @@
       <c r="B25" s="5">
         <v>20</v>
       </c>
-      <c r="C25" s="12" t="s">
+      <c r="C25" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D25" s="2" t="s">
@@ -1235,15 +1241,15 @@
       <c r="F25" s="2">
         <v>8</v>
       </c>
-      <c r="G25" s="10" t="s">
+      <c r="G25" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B26" s="15">
+      <c r="B26" s="12">
         <v>21</v>
       </c>
-      <c r="C26" s="12" t="s">
+      <c r="C26" s="20" t="s">
         <v>32</v>
       </c>
       <c r="D26" s="2" t="s">
@@ -1255,15 +1261,15 @@
       <c r="F26" s="2">
         <v>6</v>
       </c>
-      <c r="G26" s="10" t="s">
+      <c r="G26" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B27" s="15">
+      <c r="B27" s="12">
         <v>22</v>
       </c>
-      <c r="C27" s="12" t="s">
+      <c r="C27" s="20" t="s">
         <v>34</v>
       </c>
       <c r="D27" s="2" t="s">
@@ -1275,15 +1281,15 @@
       <c r="F27" s="2">
         <v>8</v>
       </c>
-      <c r="G27" s="17" t="s">
+      <c r="G27" s="14" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B28" s="15">
+      <c r="B28" s="12">
         <v>23</v>
       </c>
-      <c r="C28" s="12" t="s">
+      <c r="C28" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D28" s="2" t="s">
@@ -1295,18 +1301,18 @@
       <c r="F28" s="2">
         <v>8</v>
       </c>
-      <c r="G28" s="17" t="s">
+      <c r="G28" s="14" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B29" s="15">
+      <c r="B29" s="12">
         <v>24</v>
       </c>
-      <c r="C29" s="18" t="s">
+      <c r="C29" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="D29" s="15" t="s">
+      <c r="D29" s="12" t="s">
         <v>12</v>
       </c>
       <c r="E29" s="2">
@@ -1315,64 +1321,64 @@
       <c r="F29" s="2">
         <v>8</v>
       </c>
-      <c r="G29" s="17" t="s">
+      <c r="G29" s="14" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="15">
+      <c r="B30" s="12">
         <v>25</v>
       </c>
-      <c r="C30" s="18" t="s">
+      <c r="C30" s="22" t="s">
         <v>36</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E30" s="15">
+      <c r="E30" s="12">
         <v>24</v>
       </c>
-      <c r="F30" s="15">
+      <c r="F30" s="12">
         <v>24</v>
       </c>
-      <c r="G30" s="17" t="s">
+      <c r="G30" s="14" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B31" s="15">
+      <c r="B31" s="12">
         <v>26</v>
       </c>
-      <c r="C31" s="12" t="s">
+      <c r="C31" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E31" s="15">
+      <c r="E31" s="12">
         <v>24</v>
       </c>
-      <c r="F31" s="15">
+      <c r="F31" s="12">
         <v>24</v>
       </c>
-      <c r="G31" s="17" t="s">
+      <c r="G31" s="14" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="34" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="E34" s="19" t="s">
+      <c r="E34" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="F34" s="20" t="s">
+      <c r="F34" s="17" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="35" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="E35" s="18">
+      <c r="E35" s="15">
         <f>SUM(E6:E31)</f>
         <v>225</v>
       </c>
-      <c r="F35" s="18">
+      <c r="F35" s="15">
         <f>SUM(F6:F31)</f>
         <v>222</v>
       </c>
@@ -1411,15 +1417,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100A324A7E06DE772489F05F43B0D20114C" ma:contentTypeVersion="15" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="4b4e494e3975ca50b8e8f2bd57dce142">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3730db29-d9dc-4ee6-8792-ab0855b04f7e" xmlns:ns3="68160b8e-e5bc-4418-bf9f-9a5ebea53c19" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="99675d1f20f815f6765454f49bfd3588" ns2:_="" ns3:_="">
     <xsd:import namespace="3730db29-d9dc-4ee6-8792-ab0855b04f7e"/>
@@ -1654,15 +1651,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8A13CE6E-B686-4C1D-8D65-9440788C1B1A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DEE44FD0-6A2C-4938-9B63-1526A09B7C17}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1679,4 +1677,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8A13CE6E-B686-4C1D-8D65-9440788C1B1A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Projektdoku und Marketingdoku wurden erstellt
</commit_message>
<xml_diff>
--- a/Docs/Zeichnungen/Projektzeitplan.xlsx
+++ b/Docs/Zeichnungen/Projektzeitplan.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="44">
   <si>
     <t>Projekt Start:</t>
   </si>
@@ -53,12 +53,6 @@
   </si>
   <si>
     <t>Alle</t>
-  </si>
-  <si>
-    <t>Nicht gestartet</t>
-  </si>
-  <si>
-    <t>In Arbeit</t>
   </si>
   <si>
     <t>Fertig</t>
@@ -236,7 +230,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -257,19 +251,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -329,7 +311,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -351,63 +333,47 @@
     <xf numFmtId="14" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <color theme="5" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color theme="5" tint="-0.24994659260841701"/>
@@ -739,19 +705,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" showWhiteSpace="0" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.140625" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" customWidth="1"/>
-    <col min="3" max="3" width="51.7109375" customWidth="1"/>
-    <col min="4" max="4" width="27" customWidth="1"/>
-    <col min="5" max="5" width="24.28515625" customWidth="1"/>
-    <col min="6" max="6" width="21.28515625" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" customWidth="1"/>
+    <col min="1" max="1" width="2.5703125" customWidth="1"/>
+    <col min="2" max="2" width="6.5703125" customWidth="1"/>
+    <col min="3" max="3" width="48.7109375" customWidth="1"/>
+    <col min="4" max="4" width="22.85546875" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -767,10 +733,10 @@
       <c r="A2" s="1"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="11">
+      <c r="E2" s="10">
         <f>DATE(2025,2,3)</f>
         <v>45691</v>
       </c>
@@ -782,7 +748,7 @@
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
       <c r="D3" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E3" s="8">
         <f>DATE(2025,3,21)</f>
@@ -798,11 +764,11 @@
       <c r="D4" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
+      <c r="E4" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
@@ -810,16 +776,16 @@
         <v>2</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>3</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>4</v>
@@ -830,11 +796,11 @@
       <c r="B6" s="2">
         <v>1</v>
       </c>
-      <c r="C6" s="20" t="s">
-        <v>17</v>
+      <c r="C6" s="16" t="s">
+        <v>15</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E6" s="2">
         <v>8</v>
@@ -842,8 +808,8 @@
       <c r="F6" s="2">
         <v>8</v>
       </c>
-      <c r="G6" s="13" t="s">
-        <v>8</v>
+      <c r="G6" s="12" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -851,11 +817,11 @@
       <c r="B7" s="2">
         <v>2</v>
       </c>
-      <c r="C7" s="20" t="s">
-        <v>18</v>
+      <c r="C7" s="16" t="s">
+        <v>16</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E7" s="2">
         <v>8</v>
@@ -863,8 +829,8 @@
       <c r="F7" s="2">
         <v>6</v>
       </c>
-      <c r="G7" s="13" t="s">
-        <v>8</v>
+      <c r="G7" s="12" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -872,11 +838,11 @@
       <c r="B8" s="2">
         <v>3</v>
       </c>
-      <c r="C8" s="20" t="s">
-        <v>19</v>
+      <c r="C8" s="16" t="s">
+        <v>17</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E8" s="2">
         <v>7</v>
@@ -884,8 +850,8 @@
       <c r="F8" s="2">
         <v>7</v>
       </c>
-      <c r="G8" s="13" t="s">
-        <v>8</v>
+      <c r="G8" s="12" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -893,11 +859,11 @@
       <c r="B9" s="2">
         <v>4</v>
       </c>
-      <c r="C9" s="20" t="s">
-        <v>20</v>
+      <c r="C9" s="16" t="s">
+        <v>18</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E9" s="2">
         <v>8</v>
@@ -905,8 +871,8 @@
       <c r="F9" s="2">
         <v>7</v>
       </c>
-      <c r="G9" s="13" t="s">
-        <v>8</v>
+      <c r="G9" s="12" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -914,11 +880,11 @@
       <c r="B10" s="2">
         <v>5</v>
       </c>
-      <c r="C10" s="20" t="s">
-        <v>21</v>
+      <c r="C10" s="16" t="s">
+        <v>19</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E10" s="2">
         <v>8</v>
@@ -926,8 +892,8 @@
       <c r="F10" s="2">
         <v>6</v>
       </c>
-      <c r="G10" s="13" t="s">
-        <v>8</v>
+      <c r="G10" s="12" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -935,11 +901,11 @@
       <c r="B11" s="2">
         <v>6</v>
       </c>
-      <c r="C11" s="20" t="s">
-        <v>22</v>
+      <c r="C11" s="16" t="s">
+        <v>20</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E11" s="2">
         <v>7</v>
@@ -947,8 +913,8 @@
       <c r="F11" s="2">
         <v>7</v>
       </c>
-      <c r="G11" s="13" t="s">
-        <v>8</v>
+      <c r="G11" s="12" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -956,11 +922,11 @@
       <c r="B12" s="2">
         <v>7</v>
       </c>
-      <c r="C12" s="20" t="s">
-        <v>23</v>
+      <c r="C12" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E12" s="2">
         <v>7</v>
@@ -968,8 +934,8 @@
       <c r="F12" s="2">
         <v>6</v>
       </c>
-      <c r="G12" s="13" t="s">
-        <v>8</v>
+      <c r="G12" s="12" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -977,11 +943,11 @@
       <c r="B13" s="2">
         <v>8</v>
       </c>
-      <c r="C13" s="20" t="s">
-        <v>24</v>
+      <c r="C13" s="16" t="s">
+        <v>22</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E13" s="2">
         <v>8</v>
@@ -989,8 +955,8 @@
       <c r="F13" s="2">
         <v>8</v>
       </c>
-      <c r="G13" s="13" t="s">
-        <v>8</v>
+      <c r="G13" s="12" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -998,11 +964,11 @@
       <c r="B14" s="2">
         <v>9</v>
       </c>
-      <c r="C14" s="20" t="s">
-        <v>25</v>
+      <c r="C14" s="16" t="s">
+        <v>23</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E14" s="2">
         <v>5</v>
@@ -1010,8 +976,8 @@
       <c r="F14" s="2">
         <v>5</v>
       </c>
-      <c r="G14" s="13" t="s">
-        <v>8</v>
+      <c r="G14" s="12" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -1019,11 +985,11 @@
       <c r="B15" s="2">
         <v>10</v>
       </c>
-      <c r="C15" s="20" t="s">
-        <v>26</v>
+      <c r="C15" s="16" t="s">
+        <v>24</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E15" s="2">
         <v>7</v>
@@ -1031,8 +997,8 @@
       <c r="F15" s="2">
         <v>7</v>
       </c>
-      <c r="G15" s="13" t="s">
-        <v>8</v>
+      <c r="G15" s="12" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -1040,11 +1006,11 @@
       <c r="B16" s="2">
         <v>11</v>
       </c>
-      <c r="C16" s="20" t="s">
-        <v>27</v>
+      <c r="C16" s="16" t="s">
+        <v>25</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E16" s="2">
         <v>7</v>
@@ -1052,8 +1018,8 @@
       <c r="F16" s="2">
         <v>8</v>
       </c>
-      <c r="G16" s="13" t="s">
-        <v>8</v>
+      <c r="G16" s="12" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1061,11 +1027,11 @@
       <c r="B17" s="2">
         <v>12</v>
       </c>
-      <c r="C17" s="20" t="s">
-        <v>45</v>
+      <c r="C17" s="16" t="s">
+        <v>43</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E17" s="2">
         <v>4</v>
@@ -1073,8 +1039,8 @@
       <c r="F17" s="2">
         <v>6</v>
       </c>
-      <c r="G17" s="13" t="s">
-        <v>8</v>
+      <c r="G17" s="12" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1082,11 +1048,11 @@
       <c r="B18" s="2">
         <v>13</v>
       </c>
-      <c r="C18" s="20" t="s">
-        <v>29</v>
+      <c r="C18" s="16" t="s">
+        <v>27</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E18" s="2">
         <v>8</v>
@@ -1094,8 +1060,8 @@
       <c r="F18" s="2">
         <v>8</v>
       </c>
-      <c r="G18" s="9" t="s">
-        <v>7</v>
+      <c r="G18" s="12" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -1103,11 +1069,11 @@
       <c r="B19" s="2">
         <v>14</v>
       </c>
-      <c r="C19" s="20" t="s">
-        <v>30</v>
+      <c r="C19" s="16" t="s">
+        <v>28</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E19" s="2">
         <v>8</v>
@@ -1115,8 +1081,8 @@
       <c r="F19" s="2">
         <v>8</v>
       </c>
-      <c r="G19" s="9" t="s">
-        <v>7</v>
+      <c r="G19" s="12" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -1124,11 +1090,11 @@
       <c r="B20" s="2">
         <v>15</v>
       </c>
-      <c r="C20" s="20" t="s">
-        <v>40</v>
+      <c r="C20" s="16" t="s">
+        <v>38</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E20" s="2">
         <v>8</v>
@@ -1136,8 +1102,8 @@
       <c r="F20" s="2">
         <v>8</v>
       </c>
-      <c r="G20" s="9" t="s">
-        <v>7</v>
+      <c r="G20" s="12" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -1145,11 +1111,11 @@
       <c r="B21" s="2">
         <v>16</v>
       </c>
-      <c r="C21" s="21" t="s">
-        <v>41</v>
+      <c r="C21" s="17" t="s">
+        <v>39</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E21" s="2">
         <v>8</v>
@@ -1157,8 +1123,8 @@
       <c r="F21" s="2">
         <v>8</v>
       </c>
-      <c r="G21" s="9" t="s">
-        <v>7</v>
+      <c r="G21" s="12" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -1166,11 +1132,11 @@
       <c r="B22" s="2">
         <v>17</v>
       </c>
-      <c r="C22" s="20" t="s">
-        <v>42</v>
+      <c r="C22" s="16" t="s">
+        <v>40</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E22" s="2">
         <v>8</v>
@@ -1178,8 +1144,8 @@
       <c r="F22" s="2">
         <v>8</v>
       </c>
-      <c r="G22" s="9" t="s">
-        <v>7</v>
+      <c r="G22" s="12" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -1187,11 +1153,11 @@
       <c r="B23" s="2">
         <v>18</v>
       </c>
-      <c r="C23" s="20" t="s">
-        <v>43</v>
+      <c r="C23" s="16" t="s">
+        <v>41</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E23" s="2">
         <v>8</v>
@@ -1199,8 +1165,8 @@
       <c r="F23" s="2">
         <v>7</v>
       </c>
-      <c r="G23" s="9" t="s">
-        <v>7</v>
+      <c r="G23" s="12" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -1208,11 +1174,11 @@
       <c r="B24" s="2">
         <v>19</v>
       </c>
-      <c r="C24" s="20" t="s">
-        <v>44</v>
+      <c r="C24" s="16" t="s">
+        <v>42</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E24" s="2">
         <v>8</v>
@@ -1220,8 +1186,8 @@
       <c r="F24" s="2">
         <v>8</v>
       </c>
-      <c r="G24" s="9" t="s">
-        <v>7</v>
+      <c r="G24" s="12" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -1229,51 +1195,51 @@
       <c r="B25" s="5">
         <v>20</v>
       </c>
-      <c r="C25" s="20" t="s">
-        <v>31</v>
+      <c r="C25" s="16" t="s">
+        <v>29</v>
       </c>
       <c r="D25" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E25" s="2">
+        <v>8</v>
+      </c>
+      <c r="F25" s="2">
+        <v>8</v>
+      </c>
+      <c r="G25" s="12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B26" s="11">
+        <v>21</v>
+      </c>
+      <c r="C26" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E26" s="2">
+        <v>6</v>
+      </c>
+      <c r="F26" s="2">
+        <v>6</v>
+      </c>
+      <c r="G26" s="12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B27" s="11">
+        <v>22</v>
+      </c>
+      <c r="C27" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D27" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="E25" s="2">
-        <v>8</v>
-      </c>
-      <c r="F25" s="2">
-        <v>8</v>
-      </c>
-      <c r="G25" s="9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B26" s="12">
-        <v>21</v>
-      </c>
-      <c r="C26" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E26" s="2">
-        <v>6</v>
-      </c>
-      <c r="F26" s="2">
-        <v>6</v>
-      </c>
-      <c r="G26" s="9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B27" s="12">
-        <v>22</v>
-      </c>
-      <c r="C27" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="E27" s="2">
         <v>7</v>
@@ -1281,39 +1247,39 @@
       <c r="F27" s="2">
         <v>8</v>
       </c>
-      <c r="G27" s="14" t="s">
+      <c r="G27" s="12" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B28" s="12">
+      <c r="B28" s="11">
         <v>23</v>
       </c>
-      <c r="C28" s="20" t="s">
+      <c r="C28" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E28" s="2">
+        <v>8</v>
+      </c>
+      <c r="F28" s="2">
+        <v>8</v>
+      </c>
+      <c r="G28" s="12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B29" s="11">
+        <v>24</v>
+      </c>
+      <c r="C29" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="D28" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E28" s="2">
-        <v>8</v>
-      </c>
-      <c r="F28" s="2">
-        <v>8</v>
-      </c>
-      <c r="G28" s="14" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B29" s="12">
-        <v>24</v>
-      </c>
-      <c r="C29" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="D29" s="12" t="s">
-        <v>12</v>
+      <c r="D29" s="11" t="s">
+        <v>10</v>
       </c>
       <c r="E29" s="2">
         <v>8</v>
@@ -1321,64 +1287,64 @@
       <c r="F29" s="2">
         <v>8</v>
       </c>
-      <c r="G29" s="14" t="s">
+      <c r="G29" s="12" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="12">
+      <c r="B30" s="11">
         <v>25</v>
       </c>
-      <c r="C30" s="22" t="s">
-        <v>36</v>
+      <c r="C30" s="18" t="s">
+        <v>34</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E30" s="12">
+      <c r="E30" s="11">
         <v>24</v>
       </c>
-      <c r="F30" s="12">
+      <c r="F30" s="11">
         <v>24</v>
       </c>
-      <c r="G30" s="14" t="s">
+      <c r="G30" s="12" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B31" s="12">
+      <c r="B31" s="11">
         <v>26</v>
       </c>
-      <c r="C31" s="20" t="s">
-        <v>33</v>
+      <c r="C31" s="16" t="s">
+        <v>31</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E31" s="12">
+      <c r="E31" s="11">
         <v>24</v>
       </c>
-      <c r="F31" s="12">
+      <c r="F31" s="11">
         <v>24</v>
       </c>
-      <c r="G31" s="14" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="34" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="E34" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="F34" s="17" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="35" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="E35" s="15">
+      <c r="G31" s="12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E32" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="F32" s="15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="33" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="E33" s="13">
         <f>SUM(E6:E31)</f>
         <v>225</v>
       </c>
-      <c r="F35" s="15">
+      <c r="F33" s="13">
         <f>SUM(F6:F31)</f>
         <v>222</v>
       </c>
@@ -1390,20 +1356,15 @@
     </row>
   </sheetData>
   <protectedRanges>
-    <protectedRange sqref="E45:F45 E25:F29 C31:D31 D30 G25:G31 C25:D28 C6:G24" name="Projektdaten"/>
+    <protectedRange sqref="E45:F45 E25:F29 C31:D31 D30 C25:D28 C6:G22 C23:F24 G23:G31" name="Projektdaten"/>
     <protectedRange sqref="E3:E4" name="Stammdaten"/>
   </protectedRanges>
   <mergeCells count="1">
     <mergeCell ref="E4:G4"/>
   </mergeCells>
-  <conditionalFormatting sqref="G6:G30">
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Blockiert">
+  <conditionalFormatting sqref="G6:G31">
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="Blockiert">
       <formula>NOT(ISERROR(SEARCH("Blockiert",G6)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G31">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Blockiert">
-      <formula>NOT(ISERROR(SEARCH("Blockiert",G31)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
@@ -1412,11 +1373,20 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100A324A7E06DE772489F05F43B0D20114C" ma:contentTypeVersion="15" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="4b4e494e3975ca50b8e8f2bd57dce142">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3730db29-d9dc-4ee6-8792-ab0855b04f7e" xmlns:ns3="68160b8e-e5bc-4418-bf9f-9a5ebea53c19" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="99675d1f20f815f6765454f49bfd3588" ns2:_="" ns3:_="">
     <xsd:import namespace="3730db29-d9dc-4ee6-8792-ab0855b04f7e"/>
@@ -1651,16 +1621,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8A13CE6E-B686-4C1D-8D65-9440788C1B1A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DEE44FD0-6A2C-4938-9B63-1526A09B7C17}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1677,12 +1646,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8A13CE6E-B686-4C1D-8D65-9440788C1B1A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>